<commit_message>
Update packages for node 16
</commit_message>
<xml_diff>
--- a/statistics-runs/balancing-progress.xlsx
+++ b/statistics-runs/balancing-progress.xlsx
@@ -8,17 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\astaria-bot-backend\statistics-runs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4704A34B-6C7E-44D2-984B-BAD4FA29EC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3928CC3-BCB4-4A47-86E8-CD9DB7138824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="statistics" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>paragon</t>
   </si>
@@ -93,6 +89,9 @@
   <si>
     <t>10</t>
   </si>
+  <si>
+    <t>11</t>
+  </si>
 </sst>
 </file>
 
@@ -140,7 +139,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="18">
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
@@ -202,112 +207,1028 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="0"/>
-      <sheetName val="0-statistics"/>
-      <sheetName val="1"/>
-      <sheetName val="1-statistics"/>
-      <sheetName val="statistics"/>
-      <sheetName val="paragon"/>
-      <sheetName val="highlander"/>
-      <sheetName val="druid"/>
-      <sheetName val="oracle"/>
-      <sheetName val="avatar"/>
-      <sheetName val="shadow"/>
-      <sheetName val="lightbringer"/>
-      <sheetName val="avenger"/>
-      <sheetName val="statistics-run-9"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Harmonic Mean Statistics</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> for Heroes  (50% - optimal)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>statistics!$B$1:$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>statistics!$B$10:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.47738475057473262</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4720533542335929</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4860294999209443</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.47980102206747616</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.48317135788624044</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.488134948680715</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4879494295503648</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.48821563820912017</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.49430516754470855</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D277-4D1D-8205-579CAB505A0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="565676336"/>
+        <c:axId val="565677584"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="565676336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="565677584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="565677584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="565676336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="0"/>
-      <sheetName val="0-statistics"/>
-      <sheetName val="1"/>
-      <sheetName val="1-statistics"/>
-      <sheetName val="statistics"/>
-      <sheetName val="paragon"/>
-      <sheetName val="highlander"/>
-      <sheetName val="druid"/>
-      <sheetName val="oracle"/>
-      <sheetName val="avatar"/>
-      <sheetName val="shadow"/>
-      <sheetName val="lightbringer"/>
-      <sheetName val="avenger"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E25CE67D-A549-4D44-AC5B-8448B72090F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C92414E-A68B-46C0-9038-8C20E897643C}" name="Table1" displayName="Table1" ref="A1:I10" totalsRowCount="1">
-  <autoFilter ref="A1:I9" xr:uid="{3C92414E-A68B-46C0-9038-8C20E897643C}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C92414E-A68B-46C0-9038-8C20E897643C}" name="Table1" displayName="Table1" ref="A1:J10" totalsRowCount="1">
+  <autoFilter ref="A1:J9" xr:uid="{3C92414E-A68B-46C0-9038-8C20E897643C}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{9054F665-F68F-4619-8BF9-CF17D0E63C21}" name="hero" totalsRowLabel="Harmonic Mean"/>
-    <tableColumn id="2" xr3:uid="{C779B0F3-DD15-4C02-84FF-4B5F8E50E9B6}" name="3" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="7">
+    <tableColumn id="2" xr3:uid="{C779B0F3-DD15-4C02-84FF-4B5F8E50E9B6}" name="3" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="12">
       <totalsRowFormula>HARMEAN(Table1[3])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DAA2685D-29F8-4FA4-806C-524C3483B419}" name="4" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="6">
+    <tableColumn id="3" xr3:uid="{DAA2685D-29F8-4FA4-806C-524C3483B419}" name="4" totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="11">
       <totalsRowFormula>HARMEAN(Table1[4])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3EA211BC-96BD-47C1-B011-CCDDF6DE02D1}" name="5" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="5">
+    <tableColumn id="4" xr3:uid="{3EA211BC-96BD-47C1-B011-CCDDF6DE02D1}" name="5" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="10">
       <totalsRowFormula>HARMEAN(Table1[5])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{ABB36BA0-6F9D-4DFA-B21B-3F77DAEADBE6}" name="6" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="4">
+    <tableColumn id="5" xr3:uid="{ABB36BA0-6F9D-4DFA-B21B-3F77DAEADBE6}" name="6" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="9">
       <totalsRowFormula>HARMEAN(Table1[6])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{1997867E-3D36-4B08-A859-4A330E6CA4EB}" name="7" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="3">
+    <tableColumn id="6" xr3:uid="{1997867E-3D36-4B08-A859-4A330E6CA4EB}" name="7" totalsRowFunction="custom" dataDxfId="13" totalsRowDxfId="8">
       <totalsRowFormula>HARMEAN(Table1[7])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F03F17E2-B4C5-49FA-B50D-6CDBA7D1DB29}" name="8" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="2">
+    <tableColumn id="7" xr3:uid="{F03F17E2-B4C5-49FA-B50D-6CDBA7D1DB29}" name="8" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="7">
       <totalsRowFormula>HARMEAN(Table1[8])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{96FF3877-5217-46B6-A305-24B1C092CAD3}" name="9" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="1">
-      <calculatedColumnFormula>[1]!Table4[[#This Row],[wins]]/[1]!Table4[[#This Row],[battles]]</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{96FF3877-5217-46B6-A305-24B1C092CAD3}" name="9" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="6">
       <totalsRowFormula>HARMEAN(Table1[9])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{635C965A-57D4-4A00-9304-02A19D4343CC}" name="10" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="0">
-      <calculatedColumnFormula>[2]!Table4[[#This Row],[wins]]/[2]!Table4[[#This Row],[battles]]</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{635C965A-57D4-4A00-9304-02A19D4343CC}" name="10" totalsRowFunction="custom" dataDxfId="0" totalsRowDxfId="5">
       <totalsRowFormula>HARMEAN(Table1[10])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{ADFF34E1-BE0E-498F-B381-93415F858FA2}" name="11" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="4">
+      <totalsRowFormula>HARMEAN(Table1[11])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -577,19 +1498,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="9" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -617,8 +1538,11 @@
       <c r="I1" t="s">
         <v>17</v>
       </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -641,15 +1565,16 @@
         <v>0.62222222222222223</v>
       </c>
       <c r="H2" s="1">
-        <f>[1]!Table4[[#This Row],[wins]]/[1]!Table4[[#This Row],[battles]]</f>
         <v>0.60952380952380958</v>
       </c>
       <c r="I2" s="1">
-        <f>[2]!Table4[[#This Row],[wins]]/[2]!Table4[[#This Row],[battles]]</f>
         <v>0.65079365079365081</v>
       </c>
+      <c r="J2" s="1">
+        <v>0.61904761904761907</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -672,15 +1597,16 @@
         <v>0.48253968253968255</v>
       </c>
       <c r="H3" s="1">
-        <f>[1]!Table4[[#This Row],[wins]]/[1]!Table4[[#This Row],[battles]]</f>
         <v>0.55873015873015874</v>
       </c>
       <c r="I3" s="1">
-        <f>[2]!Table4[[#This Row],[wins]]/[2]!Table4[[#This Row],[battles]]</f>
         <v>0.53968253968253965</v>
       </c>
+      <c r="J3" s="1">
+        <v>0.52380952380952384</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -703,15 +1629,16 @@
         <v>0.43492063492063493</v>
       </c>
       <c r="H4" s="1">
-        <f>[1]!Table4[[#This Row],[wins]]/[1]!Table4[[#This Row],[battles]]</f>
         <v>0.43809523809523809</v>
       </c>
       <c r="I4" s="1">
-        <f>[2]!Table4[[#This Row],[wins]]/[2]!Table4[[#This Row],[battles]]</f>
         <v>0.44126984126984126</v>
       </c>
+      <c r="J4" s="1">
+        <v>0.43492063492063493</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -734,15 +1661,16 @@
         <v>0.46031746031746029</v>
       </c>
       <c r="H5" s="1">
-        <f>[1]!Table4[[#This Row],[wins]]/[1]!Table4[[#This Row],[battles]]</f>
         <v>0.4507936507936508</v>
       </c>
       <c r="I5" s="1">
-        <f>[2]!Table4[[#This Row],[wins]]/[2]!Table4[[#This Row],[battles]]</f>
         <v>0.43174603174603177</v>
       </c>
+      <c r="J5" s="1">
+        <v>0.49523809523809526</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -765,15 +1693,16 @@
         <v>0.43809523809523809</v>
       </c>
       <c r="H6" s="1">
-        <f>[1]!Table4[[#This Row],[wins]]/[1]!Table4[[#This Row],[battles]]</f>
         <v>0.40317460317460319</v>
       </c>
       <c r="I6" s="1">
-        <f>[2]!Table4[[#This Row],[wins]]/[2]!Table4[[#This Row],[battles]]</f>
         <v>0.46666666666666667</v>
       </c>
+      <c r="J6" s="1">
+        <v>0.44444444444444442</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -796,15 +1725,16 @@
         <v>0.54603174603174598</v>
       </c>
       <c r="H7" s="1">
-        <f>[1]!Table4[[#This Row],[wins]]/[1]!Table4[[#This Row],[battles]]</f>
         <v>0.60952380952380958</v>
       </c>
       <c r="I7" s="1">
-        <f>[2]!Table4[[#This Row],[wins]]/[2]!Table4[[#This Row],[battles]]</f>
         <v>0.50476190476190474</v>
       </c>
+      <c r="J7" s="1">
+        <v>0.48571428571428571</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -827,15 +1757,16 @@
         <v>0.4</v>
       </c>
       <c r="H8" s="1">
-        <f>[1]!Table4[[#This Row],[wins]]/[1]!Table4[[#This Row],[battles]]</f>
         <v>0.41904761904761906</v>
       </c>
       <c r="I8" s="1">
-        <f>[2]!Table4[[#This Row],[wins]]/[2]!Table4[[#This Row],[battles]]</f>
         <v>0.39365079365079364</v>
       </c>
+      <c r="J8" s="1">
+        <v>0.46349206349206351</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -858,15 +1789,16 @@
         <v>0.61587301587301591</v>
       </c>
       <c r="H9" s="1">
-        <f>[1]!Table4[[#This Row],[wins]]/[1]!Table4[[#This Row],[battles]]</f>
         <v>0.51111111111111107</v>
       </c>
       <c r="I9" s="1">
-        <f>[2]!Table4[[#This Row],[wins]]/[2]!Table4[[#This Row],[battles]]</f>
         <v>0.5714285714285714</v>
       </c>
+      <c r="J9" s="1">
+        <v>0.53333333333333333</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -901,11 +1833,55 @@
       <c r="I10" s="1">
         <f>HARMEAN(Table1[10])</f>
         <v>0.48821563820912017</v>
+      </c>
+      <c r="J10" s="1">
+        <f>HARMEAN(Table1[11])</f>
+        <v>0.49430516754470855</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:B9">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C9">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D9">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E9">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F9">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -915,7 +1891,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C9">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -925,55 +1901,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D9">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E9">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F9">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B10:I10">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
+  <conditionalFormatting sqref="B10:J10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -984,8 +1912,26 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H9">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -995,7 +1941,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="J2:J9">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1006,8 +1952,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>